<commit_message>
update sample_efficiency to 31
</commit_message>
<xml_diff>
--- a/sample_efficiency/sample_eff_benchmark.xlsx
+++ b/sample_efficiency/sample_eff_benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacky\Desktop\results\sample_efficiency\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A750D8A-545F-4969-B12C-8D7E9F0F678B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2257A741-3FBF-4252-A329-BC05219552F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13635" yWindow="3420" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Ray: </t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>47.11 seconds</t>
+  </si>
+  <si>
+    <t>35.44 seconds</t>
+  </si>
+  <si>
+    <t>33.04 seconds</t>
+  </si>
+  <si>
+    <t>32.88 seconds</t>
   </si>
 </sst>
 </file>
@@ -372,7 +381,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,6 +410,15 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>